<commit_message>
updates to results and discussion
</commit_message>
<xml_diff>
--- a/figures/Figures.xlsx
+++ b/figures/Figures.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="EDS plots" sheetId="2" r:id="rId2"/>
+    <sheet name="C1 AR EDS" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Element</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Ni</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Spot A large carbide</t>
+  </si>
+  <si>
+    <t>Spot B aggregate particles</t>
   </si>
 </sst>
 </file>
@@ -154,8 +166,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1369219" y="366713"/>
-          <a:ext cx="5097065" cy="3214687"/>
+          <a:off x="1371600" y="371475"/>
+          <a:ext cx="5105400" cy="3257550"/>
           <a:chOff x="1214438" y="390525"/>
           <a:chExt cx="4555331" cy="3429000"/>
         </a:xfrm>
@@ -402,8 +414,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7530703" y="357188"/>
-          <a:ext cx="5097066" cy="3214687"/>
+          <a:off x="7543800" y="361950"/>
+          <a:ext cx="5105400" cy="3257550"/>
           <a:chOff x="6679406" y="381000"/>
           <a:chExt cx="4555332" cy="3429000"/>
         </a:xfrm>
@@ -679,6 +691,45 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3657600" cy="2491564"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="4248152"/>
+          <a:ext cx="3657600" cy="2491564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1018,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B16:D40"/>
+  <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1035,8 +1086,13 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="16" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1058,7 +1114,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1069,7 +1125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1091,16 +1147,89 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="4"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+    <row r="22" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="5">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="5">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21</v>
+      </c>
+      <c r="D43" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>16</v>
+      </c>
+      <c r="D44" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more updates to Results and Discussion
</commit_message>
<xml_diff>
--- a/figures/Figures.xlsx
+++ b/figures/Figures.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MJGroup\Documents\GitHub\MS-Thesis\figures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="20115" windowHeight="11055" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="C1 AR EDS" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="_xltb_storage_" sheetId="5" state="veryHidden" r:id="rId4"/>
+    <sheet name="C1 AR EDS new" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="C5 AR EDS" sheetId="7" r:id="rId7"/>
+    <sheet name="C1 OH 2375 EDS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="18">
   <si>
     <t>Element</t>
   </si>
@@ -50,11 +60,41 @@
   <si>
     <t>Spot B aggregate particles</t>
   </si>
+  <si>
+    <t>XL Toolbox Settings</t>
+  </si>
+  <si>
+    <t>export_preset</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;_x000D_
+&lt;Preset xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema"&gt;_x000D_
+  &lt;Name&gt;Png, 300 dpi, RGB, Transparent canvas&lt;/Name&gt;_x000D_
+  &lt;Dpi&gt;300&lt;/Dpi&gt;_x000D_
+  &lt;FileType&gt;Png&lt;/FileType&gt;_x000D_
+  &lt;ColorSpace&gt;Rgb&lt;/ColorSpace&gt;_x000D_
+  &lt;Transparency&gt;TransparentCanvas&lt;/Transparency&gt;_x000D_
+  &lt;UseColorProfile&gt;false&lt;/UseColorProfile&gt;_x000D_
+  &lt;ColorProfile&gt;2007FP&lt;/ColorProfile&gt;_x000D_
+&lt;/Preset&gt;</t>
+  </si>
+  <si>
+    <t>export_path</t>
+  </si>
+  <si>
+    <t>Spot B particles at periphery</t>
+  </si>
+  <si>
+    <t>Liquated region</t>
+  </si>
+  <si>
+    <t>C:\Users\MJGroup\Documents\GitHub\MS-Thesis\figures\metallography\c1-oh-2375-liquation-sem.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -123,6 +163,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -139,6 +197,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -733,6 +794,384 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157942</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="219077"/>
+          <a:ext cx="3657600" cy="2491565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3657600" cy="2491564"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="4248152"/>
+          <a:ext cx="3657600" cy="2491564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157941</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="219077"/>
+          <a:ext cx="3657600" cy="2491564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3657600" cy="2491564"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="4448177"/>
+          <a:ext cx="3657600" cy="2491564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>65943</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1391382</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157941</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="754805" y="216696"/>
+          <a:ext cx="3621644" cy="2467071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9153185" y="885825"/>
+          <a:ext cx="5510893" cy="4066495"/>
+          <a:chOff x="9153185" y="885825"/>
+          <a:chExt cx="5510893" cy="4066495"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="4" name="Picture 3"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9153185" y="885825"/>
+            <a:ext cx="5510893" cy="4066495"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Cross 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12439032" y="1943936"/>
+            <a:ext cx="455469" cy="449190"/>
+          </a:xfrm>
+          <a:prstGeom prst="plus">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 48121"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 5"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="12777726" y="1802947"/>
+            <a:ext cx="398318" cy="357790"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="00FF00"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1056,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1071,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1248,4 +1687,729 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="B25:H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="12.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="10.875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="F5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>96</v>
+      </c>
+      <c r="H6" s="5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>96</v>
+      </c>
+      <c r="D18" s="5">
+        <v>94</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="F28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="5">
+        <v>42</v>
+      </c>
+      <c r="H29" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="5">
+        <v>11</v>
+      </c>
+      <c r="H30" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5">
+        <v>21</v>
+      </c>
+      <c r="H31" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="5">
+        <v>16</v>
+      </c>
+      <c r="H32" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="5">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5">
+        <v>22</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="5">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21</v>
+      </c>
+      <c r="D43" s="5">
+        <v>19</v>
+      </c>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>16</v>
+      </c>
+      <c r="D44" s="5">
+        <v>13</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="12.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="10.875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="F5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>84</v>
+      </c>
+      <c r="H6" s="5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="H7" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>7</v>
+      </c>
+      <c r="H8" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="H9" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="F28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="5">
+        <v>72</v>
+      </c>
+      <c r="H29" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="5">
+        <v>7</v>
+      </c>
+      <c r="H30" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5">
+        <v>13</v>
+      </c>
+      <c r="H31" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="7">
+        <v>9</v>
+      </c>
+      <c r="H32" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="5">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5">
+        <v>22</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="5">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21</v>
+      </c>
+      <c r="D43" s="5">
+        <v>19</v>
+      </c>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>16</v>
+      </c>
+      <c r="D44" s="5">
+        <v>13</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="D46" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="H14" sqref="B2:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="12.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="10.875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="F5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>21</v>
+      </c>
+      <c r="H6" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45</v>
+      </c>
+      <c r="H8" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>